<commit_message>
SAVE MORNING 31 08 2023
sauvegarde du projet sprint 1
</commit_message>
<xml_diff>
--- a/GestionTemps.xlsx
+++ b/GestionTemps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grognone\Desktop\SaveCda\ScrumPicsou\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A090E587-2CAF-4AF3-A3C5-B8A1A7ED793B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34329351-FC60-46F8-B7E4-BBC37A1E31B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacite" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
   <si>
     <t>Capacité de travail</t>
   </si>
@@ -113,9 +113,6 @@
     <t xml:space="preserve">Le possesseur de la carte n'a accès qu'au retrait avec ou sans délivrance de reçu. </t>
   </si>
   <si>
-    <t xml:space="preserve">Le client de la banque a accès aux options de retrait avec ou sans délivrance de reçu (le reçu peut indiquer le solde du compte), dépôt, consultation de solde de ses comptes. </t>
-  </si>
-  <si>
     <t>En tant que possesseur d’une carte de retrait, je souhaite sélectionner quel montant retirer dans le but de choisir combien d'espèces obtenir</t>
   </si>
   <si>
@@ -125,16 +122,7 @@
     <t>En tant que possesseur d’une carte de retrait, je souhaite récupérer mes billets dans le but de les dépenser</t>
   </si>
   <si>
-    <t xml:space="preserve">L'écran affiche un message invitant à retirer la carte. </t>
-  </si>
-  <si>
     <t>En tant que possesseur d’une carte de retrait, je souhaite saisir quel montant retirer dans le but de choisir combien d'espèces obtenir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le client saisie le montant à retirer. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L'écran affiche un message invitant à récupérer les billets. </t>
   </si>
   <si>
     <t xml:space="preserve">En tant que possesseur d’une carte de retrait, je souhaite saisir le code secret associé à ma carte dans le but de m’identifier. </t>
@@ -156,9 +144,6 @@
   </si>
   <si>
     <t>En tant que client de la banque PICSOU, je souhaite déposer des espèces dans le but d'alimenter mon compte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le client a accès aux écrans de dépôt d'espèces, avec une invite lui demandant d'insérer ses espèces. </t>
   </si>
   <si>
     <t xml:space="preserve">Date </t>
@@ -224,6 +209,49 @@
   </si>
   <si>
     <t>SCREEN SIZE DESKTOP WIREFRAME 1440 * 1024</t>
+  </si>
+  <si>
+    <t>Etant donné que j’ai terminé l’opération de retrait 
+Lorsque j’ai retiré ma carte
+Alors je peux retirer mes billets</t>
+  </si>
+  <si>
+    <t>Etant que j’ai récupéré ma carte
+Lorsque je récupère mes billets
+Alors je peux les dépenser</t>
+  </si>
+  <si>
+    <t>Etant donné que j’ai inséré ma carte
+Lorsque j’ai saisie mon code Et qu’il est valide
+Alors je peux être identifié</t>
+  </si>
+  <si>
+    <t>Etant donné que je suis possesseur d’une carte de retrait
+Lorsque je me présente devant le distributeur Et que le message demandant à introduire la carte est présent
+Alors j’introduit la carte dans le lecteur de carte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Etant donné que je suis client de la banque PICSOU
+Lorsque je suis identifié
+Alors je peux accéder à mon espace dédié comportant les options d’opérations disponibles qui sont le retrait avec ou sans délivrance de reçu (le reçu peut indiquer le solde du compte), dépôt, consultation de solde de ses comptes. </t>
+  </si>
+  <si>
+    <t>Etant donné que je ne suis pas client de la banque PICSOU
+Lorsque je suis identifié 
+Alors le distributeur me propose d’effectuer un retrait avec ou sans reçu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Etant donné que je suis identifié en tant que client de la banque PICSOU
+Lorsque je sélectionne l’option de dépôt 
+Alors je peux déposer mon argent sur le compte choisi. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Etant donné que j’ai choisi l’option retrait d’espèces
+Lorsque j’ai saisi le montant à retirer Et que j’ai validé
+Alors je peux récupérer mes espèces correspondant au montant choisi. </t>
+  </si>
+  <si>
+    <t>IMPRESSION TICKET</t>
   </si>
 </sst>
 </file>
@@ -344,18 +372,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -780,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C26FCD31-FEA3-4BDA-92A6-38C4B0104E23}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,7 +858,7 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -839,12 +867,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C4">
         <v>120</v>
@@ -853,7 +881,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -861,7 +889,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -870,7 +898,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -878,7 +906,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>90</v>
@@ -887,7 +915,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -895,7 +923,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7">
         <v>90</v>
@@ -904,7 +932,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>56</v>
+      </c>
+      <c r="F7" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -912,7 +943,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8">
         <v>90</v>
@@ -921,15 +952,15 @@
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>90</v>
@@ -938,15 +969,15 @@
         <v>3</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10">
         <v>50</v>
@@ -955,15 +986,15 @@
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C11">
         <v>50</v>
@@ -972,15 +1003,15 @@
         <v>5</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C12">
         <v>20</v>
@@ -989,7 +1020,7 @@
         <v>4</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1015,21 +1046,21 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E18" s="2"/>
     </row>
@@ -1091,7 +1122,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>15</v>
@@ -1105,7 +1136,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C2" s="10">
         <v>120</v>
@@ -1114,10 +1145,10 @@
         <v>1</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1125,7 +1156,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C3" s="10">
         <v>100</v>
@@ -1134,7 +1165,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F3" s="18"/>
     </row>
@@ -1143,7 +1174,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="10">
         <v>90</v>
@@ -1152,7 +1183,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F4" s="18"/>
     </row>
@@ -1161,7 +1192,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C5" s="10">
         <v>90</v>
@@ -1211,28 +1242,28 @@
   <sheetData>
     <row r="1" spans="1:6" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1240,19 +1271,19 @@
         <v>45168</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1260,17 +1291,17 @@
         <v>45168</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
send 31 08 2023
</commit_message>
<xml_diff>
--- a/GestionTemps.xlsx
+++ b/GestionTemps.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grognone\Desktop\SaveCda\ScrumPicsou\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5399F4E3-91C5-4338-B2C4-38723983B17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39FB515-F9A1-4283-BD8C-47A328540C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacite" sheetId="1" r:id="rId1"/>
     <sheet name="BacklogProduit" sheetId="2" r:id="rId2"/>
-    <sheet name="BacklogSprint" sheetId="5" r:id="rId3"/>
-    <sheet name="Planification Réunions" sheetId="3" r:id="rId4"/>
+    <sheet name="BacklogSpring2" sheetId="6" r:id="rId3"/>
+    <sheet name="BacklogSprint1" sheetId="5" r:id="rId4"/>
+    <sheet name="Planification Réunions" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
   <si>
     <t>Capacité de travail</t>
   </si>
@@ -278,12 +279,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -291,6 +286,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -338,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -369,14 +370,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -799,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C26FCD31-FEA3-4BDA-92A6-38C4B0104E23}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +864,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
+      <c r="A4" s="22">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -876,7 +881,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
+      <c r="A5" s="22">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -893,7 +898,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+      <c r="A6" s="22">
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -910,7 +915,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="A7" s="14">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -927,7 +932,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="14">
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -944,7 +949,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
+      <c r="A9" s="22">
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -961,7 +966,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="A10" s="14">
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -978,7 +983,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="A11" s="14">
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -995,7 +1000,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+      <c r="A12" s="15">
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1032,21 +1037,21 @@
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
+      <c r="A16" s="22"/>
       <c r="B16" t="s">
         <v>49</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
+      <c r="A17" s="14"/>
       <c r="B17" t="s">
         <v>50</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="A18" s="15"/>
       <c r="B18" t="s">
         <v>51</v>
       </c>
@@ -1083,11 +1088,124 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B210576-E0D6-42ED-8164-B5DEE235A494}">
+  <dimension ref="A2:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="5" max="5" width="40.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="23">
+        <v>4</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="19">
+        <v>90</v>
+      </c>
+      <c r="D3" s="19">
+        <v>1</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="20"/>
+    </row>
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="23">
+        <v>5</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="19">
+        <v>90</v>
+      </c>
+      <c r="D4" s="19">
+        <v>1</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="20"/>
+    </row>
+    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="23">
+        <v>7</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="19">
+        <v>50</v>
+      </c>
+      <c r="D5" s="19">
+        <v>2</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="20"/>
+    </row>
+    <row r="6" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A6" s="23">
+        <v>8</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="19">
+        <v>50</v>
+      </c>
+      <c r="D6" s="19">
+        <v>5</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F8571B8-F310-4939-B46C-82BE6CA66E94}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,8 +1237,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
+    <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -1132,15 +1250,15 @@
       <c r="D2" s="10">
         <v>1</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -1152,13 +1270,13 @@
       <c r="D3" s="10">
         <v>2</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="18"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="A4" s="21">
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
@@ -1173,10 +1291,10 @@
       <c r="E4" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="A5" s="21">
         <v>6</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -1188,29 +1306,29 @@
       <c r="D5" s="10">
         <v>3</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="18"/>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F6" s="19"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F7" s="19"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F8" s="19"/>
+      <c r="F8" s="17"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F9" s="19"/>
+      <c r="F9" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8CFA39-DF7F-4CBB-914F-A65826EAC886}">
   <dimension ref="A1:F730"/>
   <sheetViews>

</xml_diff>

<commit_message>
send 01 09 2023
</commit_message>
<xml_diff>
--- a/GestionTemps.xlsx
+++ b/GestionTemps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grognone\Desktop\SaveCda\ScrumPicsou\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39FB515-F9A1-4283-BD8C-47A328540C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A021EF-8274-431E-A4B8-9755527BF5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacite" sheetId="1" r:id="rId1"/>
@@ -270,7 +270,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,6 +292,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -339,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -376,15 +382,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,7 +805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C26FCD31-FEA3-4BDA-92A6-38C4B0104E23}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
@@ -864,7 +865,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="22">
+      <c r="A4" s="19">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -881,7 +882,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
+      <c r="A5" s="19">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -898,7 +899,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
+      <c r="A6" s="19">
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -949,7 +950,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
+      <c r="A9" s="19">
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1037,7 +1038,7 @@
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
+      <c r="A16" s="19"/>
       <c r="B16" t="s">
         <v>49</v>
       </c>
@@ -1091,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B210576-E0D6-42ED-8164-B5DEE235A494}">
   <dimension ref="A2:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,96 +1105,96 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="23">
+      <c r="A3" s="21">
         <v>4</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="10">
         <v>90</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="10">
         <v>1</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="20"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="23">
+      <c r="A4" s="21">
         <v>5</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="10">
         <v>90</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="10">
         <v>1</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="20"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="23">
+      <c r="A5" s="21">
         <v>7</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="10">
         <v>50</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="10">
         <v>2</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="20"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A6" s="23">
+      <c r="A6" s="20">
         <v>8</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="10">
         <v>50</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="10">
         <v>5</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="20"/>
+      <c r="F6" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1238,7 +1239,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="21">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -1258,7 +1259,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="21">
+      <c r="A3" s="18">
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -1276,7 +1277,7 @@
       <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
+      <c r="A4" s="18">
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
@@ -1294,7 +1295,7 @@
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
+      <c r="A5" s="18">
         <v>6</v>
       </c>
       <c r="B5" s="13" t="s">

</xml_diff>